<commit_message>
Submitted version after review.
</commit_message>
<xml_diff>
--- a/all.xlsx
+++ b/all.xlsx
@@ -451,7 +451,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6910112359550562</v>
+        <v>0.6853932584269663</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -535,7 +535,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6067415730337079</v>
+        <v>0.6460674157303371</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -619,7 +619,7 @@
         <v>5</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5337078651685393</v>
+        <v>0.6123595505617978</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -661,7 +661,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5617977528089888</v>
+        <v>0.6235955056179775</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -703,7 +703,7 @@
         <v>5</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5674157303370787</v>
+        <v>0.6853932584269663</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -745,7 +745,7 @@
         <v>5</v>
       </c>
       <c r="D24" t="n">
-        <v>0.5449438202247191</v>
+        <v>0.6910112359550562</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -787,7 +787,7 @@
         <v>5</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5561797752808989</v>
+        <v>0.5842696629213483</v>
       </c>
     </row>
     <row r="28" spans="1:4">

</xml_diff>